<commit_message>
add scalable random weighted sampler
</commit_message>
<xml_diff>
--- a/doc/poster/scalable_random_weighted_sampler.xlsx
+++ b/doc/poster/scalable_random_weighted_sampler.xlsx
@@ -24,6 +24,15 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -250,11 +259,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-74119936"/>
-        <c:axId val="-96528288"/>
+        <c:axId val="-68915904"/>
+        <c:axId val="-68913584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-74119936"/>
+        <c:axId val="-68915904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -297,7 +306,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-96528288"/>
+        <c:crossAx val="-68913584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -305,7 +314,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-96528288"/>
+        <c:axId val="-68913584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -355,7 +364,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-74119936"/>
+        <c:crossAx val="-68915904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -573,11 +582,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-148151392"/>
-        <c:axId val="-99221184"/>
+        <c:axId val="-95694080"/>
+        <c:axId val="-68899056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-148151392"/>
+        <c:axId val="-95694080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -620,7 +629,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-99221184"/>
+        <c:crossAx val="-68899056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -628,7 +637,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-99221184"/>
+        <c:axId val="-68899056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,6 +657,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -678,7 +688,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-148151392"/>
+        <c:crossAx val="-95694080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -896,11 +906,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-98798736"/>
-        <c:axId val="-94603920"/>
+        <c:axId val="-68879968"/>
+        <c:axId val="-68877216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-98798736"/>
+        <c:axId val="-68879968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,7 +953,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-94603920"/>
+        <c:crossAx val="-68877216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -951,7 +961,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-94603920"/>
+        <c:axId val="-68877216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,7 +1011,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-98798736"/>
+        <c:crossAx val="-68879968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1095,6 +1105,14 @@
               <a:rPr lang="en-US" altLang="zh-CN"/>
               <a:t>Proportion</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>factor=0.0</a:t>
+            </a:r>
             <a:endParaRPr lang="zh-CN" altLang="en-US"/>
           </a:p>
         </c:rich>
@@ -1211,11 +1229,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-220739456"/>
-        <c:axId val="-94857648"/>
+        <c:axId val="-67981680"/>
+        <c:axId val="-67979360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-220739456"/>
+        <c:axId val="-67981680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1258,7 +1276,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-94857648"/>
+        <c:crossAx val="-67979360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1266,7 +1284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-94857648"/>
+        <c:axId val="-67979360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1316,7 +1334,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-220739456"/>
+        <c:crossAx val="-67981680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3925,85 +3943,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A59"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>373</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>575</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4929</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1083</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2039</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1138</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2152</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>338</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>170</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="Q10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>681</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1421</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>585</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>459</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>19.313207915827899</v>
       </c>

</xml_diff>